<commit_message>
completed quotation creation functional flow
</commit_message>
<xml_diff>
--- a/src/main/java/Resources/test_data_sheet.xlsx
+++ b/src/main/java/Resources/test_data_sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>customer</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Miss</t>
   </si>
   <si>
-    <t>865360920V</t>
-  </si>
-  <si>
     <t>Lilani</t>
   </si>
   <si>
@@ -76,6 +73,12 @@
   </si>
   <si>
     <t>300/A</t>
+  </si>
+  <si>
+    <t>Rajapihilla</t>
+  </si>
+  <si>
+    <t>865361920V</t>
   </si>
 </sst>
 </file>
@@ -412,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15"/>
@@ -473,18 +476,21 @@
         <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="J2" s="1">
         <v>71463764377</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added comments and test method to create quotation without customer details
</commit_message>
<xml_diff>
--- a/src/main/java/Resources/test_data_sheet.xlsx
+++ b/src/main/java/Resources/test_data_sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="98">
   <si>
     <t>customer</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>Rental</t>
+  </si>
+  <si>
+    <t>policy_start_date</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -644,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15"/>
@@ -658,11 +664,11 @@
     <col min="23" max="23" width="18.28515625" style="3"/>
     <col min="24" max="24" width="18.28515625" style="1"/>
     <col min="25" max="25" width="29.85546875" style="1" customWidth="1"/>
-    <col min="26" max="27" width="18.28515625" style="3"/>
-    <col min="28" max="16384" width="18.28515625" style="1"/>
+    <col min="26" max="28" width="18.28515625" style="3"/>
+    <col min="29" max="16384" width="18.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,8 +750,11 @@
       <c r="AA1" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="AB1" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:28">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -815,8 +824,11 @@
       <c r="AA2" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="AB2" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:28">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -886,8 +898,11 @@
       <c r="AA3" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="AB3" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -942,8 +957,11 @@
       <c r="AA4" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="AB4" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:28">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -998,8 +1016,11 @@
       <c r="AA5" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="AB5" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:28">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1054,8 +1075,11 @@
       <c r="AA6" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="AB6" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:28">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1110,8 +1134,11 @@
       <c r="AA7" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="AB7" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:28">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1166,8 +1193,11 @@
       <c r="AA8" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="AB8" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:28">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1221,10 +1251,14 @@
       </c>
       <c r="AA9" s="3" t="s">
         <v>66</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>